<commit_message>
[Task/CRA-155] Android logs file upload API (#157)
* Android logs file upload API

* android logs and students file update

* Log and student file upload API
</commit_message>
<xml_diff>
--- a/backend/studentList/Unregistered Students.xlsx
+++ b/backend/studentList/Unregistered Students.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -387,32 +387,22 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>The student (suchitra@gmail.com) is already registered</v>
+        <v>The student (suchitra2@gmail.com) is already registered</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>The student (suchitra1@gmail.com) is already registered</v>
+        <v>The student (suchitra4@gmail.com) is already registered</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>The student (suchitra2@gmail.com) is already registered</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>The student (suchitra4@gmail.com) is already registered</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
         <v>Found duplicate Roll number(1680210680), please check the data of the student suchitra3@gmail.com</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes in backend and added frontend code
</commit_message>
<xml_diff>
--- a/backend/studentList/Unregistered Students.xlsx
+++ b/backend/studentList/Unregistered Students.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -387,22 +387,72 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>The student (suchitra2@gmail.com) is already registered</v>
+        <v>"name" is required for the student undefined</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>The student (suchitra4@gmail.com) is already registered</v>
+        <v>"name" is required for the student undefined</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Found duplicate Roll number(1680210680), please check the data of the student suchitra3@gmail.com</v>
+        <v>"name" is required for the student undefined</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>"name" is required for the student undefined</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>"name" is required for the student undefined</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>"name" is required for the student undefined</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>"name" is required for the student undefined</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>"name" is required for the student undefined</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>"name" is required for the student undefined</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>"name" is required for the student undefined</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>"name" is required for the student undefined</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>"name" is required for the student undefined</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>"name" is required for the student undefined</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A14"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Backend and frontend code (#207)
* Changes in backend and added frontend code

* change in gitignore file and added frontend/src folder

* Syncing code

* add question and paper repetition

* Upload

* Initial commit

* all the repetition completed on frontend and some changed on backend

* Syncing code

* worked on tpo and admin dashboard

* Pushing student dashboard

* question paper create completed

* Student dashboard join test window

* instruction window

* Syncing code

* fetch instructions

Co-authored-by: bhardwajaditya113 <bhardwajaditya113@gmail.com>
</commit_message>
<xml_diff>
--- a/backend/studentList/Unregistered Students.xlsx
+++ b/backend/studentList/Unregistered Students.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -387,22 +387,27 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>The student (suchitra2@gmail.com) is already registered</v>
+        <v>Already registered with the email suchitra@gmail.com, try to login</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>The student (suchitra4@gmail.com) is already registered</v>
+        <v>Already registered with the email suchitra1@gmail.com, try to login</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Found duplicate Roll number(1680210680), please check the data of the student suchitra3@gmail.com</v>
+        <v>Already registered with the email suchitra2@gmail.com, try to login</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Already registered with the email suchitra4@gmail.com, try to login</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changes in backend to solve the server problem and added exam window component in frontend
</commit_message>
<xml_diff>
--- a/backend/studentList/Unregistered Students.xlsx
+++ b/backend/studentList/Unregistered Students.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -387,27 +387,72 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Already registered with the email suchitra@gmail.com, try to login</v>
+        <v>"name" is required for the student undefined</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Already registered with the email suchitra1@gmail.com, try to login</v>
+        <v>"name" is required for the student undefined</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Already registered with the email suchitra2@gmail.com, try to login</v>
+        <v>"name" is required for the student undefined</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Already registered with the email suchitra4@gmail.com, try to login</v>
+        <v>"name" is required for the student undefined</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>"name" is required for the student undefined</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>"name" is required for the student undefined</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>"name" is required for the student undefined</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>"name" is required for the student undefined</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>"name" is required for the student undefined</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>"name" is required for the student undefined</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>"name" is required for the student undefined</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>"name" is required for the student undefined</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>"name" is required for the student undefined</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A14"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>